<commit_message>
in de planning en assetlist gezed wat ik af heb
sara rig blauw gemaakt
</commit_message>
<xml_diff>
--- a/Planning/Assetlist.xlsx
+++ b/Planning/Assetlist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CarloAkuma\Desktop\JOHN CENA TUUTUUDUU TUUU\Gamelab1\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Desktop\Gamelab1\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2193,7 +2193,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2209,9 +2209,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2249,7 +2249,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2321,7 +2321,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2473,8 +2473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:CD93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="46" zoomScaleNormal="46" workbookViewId="0">
-      <selection activeCell="BI3" sqref="BI3:BI37"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="AJ3" sqref="AJ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2700,7 +2700,7 @@
         <v>307</v>
       </c>
       <c r="AI3" s="3"/>
-      <c r="AJ3" s="3" t="s">
+      <c r="AJ3" s="34" t="s">
         <v>319</v>
       </c>
       <c r="AK3" s="10"/>

</xml_diff>

<commit_message>
afgekruist wat ik af heb
het is ook verplaatst in trello
</commit_message>
<xml_diff>
--- a/Planning/Assetlist.xlsx
+++ b/Planning/Assetlist.xlsx
@@ -2473,8 +2473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:CD93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="AJ3" sqref="AJ3"/>
+    <sheetView tabSelected="1" topLeftCell="AB16" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="AU34" sqref="AU34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5941,7 +5941,7 @@
       </c>
       <c r="AS32" s="3"/>
       <c r="AT32" s="3"/>
-      <c r="AU32" s="3" t="s">
+      <c r="AU32" s="34" t="s">
         <v>383</v>
       </c>
       <c r="AV32" s="10"/>
@@ -6048,7 +6048,7 @@
       </c>
       <c r="AS33" s="3"/>
       <c r="AT33" s="3"/>
-      <c r="AU33" s="3" t="s">
+      <c r="AU33" s="34" t="s">
         <v>383</v>
       </c>
       <c r="AV33" s="10"/>
@@ -6155,7 +6155,7 @@
       </c>
       <c r="AS34" s="3"/>
       <c r="AT34" s="3"/>
-      <c r="AU34" s="3" t="s">
+      <c r="AU34" s="34" t="s">
         <v>383</v>
       </c>
       <c r="AV34" s="10"/>

</xml_diff>

<commit_message>
Woodsword en planning update
</commit_message>
<xml_diff>
--- a/Planning/Assetlist.xlsx
+++ b/Planning/Assetlist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Desktop\Gamelab1\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CarloAkuma\Desktop\JOHN CENA TUUTUUDUU TUUU\Gamelab1\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="635">
   <si>
     <t>2D</t>
   </si>
@@ -1957,6 +1957,12 @@
   </si>
   <si>
     <t>2D_ENVFB_001</t>
+  </si>
+  <si>
+    <t>7S_SAL_001</t>
+  </si>
+  <si>
+    <t>Save And Load</t>
   </si>
 </sst>
 </file>
@@ -2035,7 +2041,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2146,11 +2152,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2191,9 +2208,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2209,9 +2228,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2249,7 +2268,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2321,7 +2340,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2473,8 +2492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:CD93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB16" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="AU34" sqref="AU34"/>
+    <sheetView tabSelected="1" topLeftCell="AY20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BG38" activeCellId="1" sqref="BA38:BE38 BG38:BI38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2700,7 +2719,7 @@
         <v>307</v>
       </c>
       <c r="AI3" s="3"/>
-      <c r="AJ3" s="34" t="s">
+      <c r="AJ3" s="3" t="s">
         <v>319</v>
       </c>
       <c r="AK3" s="10"/>
@@ -5941,7 +5960,7 @@
       </c>
       <c r="AS32" s="3"/>
       <c r="AT32" s="3"/>
-      <c r="AU32" s="34" t="s">
+      <c r="AU32" s="3" t="s">
         <v>383</v>
       </c>
       <c r="AV32" s="10"/>
@@ -6048,7 +6067,7 @@
       </c>
       <c r="AS33" s="3"/>
       <c r="AT33" s="3"/>
-      <c r="AU33" s="34" t="s">
+      <c r="AU33" s="3" t="s">
         <v>383</v>
       </c>
       <c r="AV33" s="10"/>
@@ -6155,7 +6174,7 @@
       </c>
       <c r="AS34" s="3"/>
       <c r="AT34" s="3"/>
-      <c r="AU34" s="34" t="s">
+      <c r="AU34" s="3" t="s">
         <v>383</v>
       </c>
       <c r="AV34" s="10"/>
@@ -6590,6 +6609,22 @@
       </c>
       <c r="AX38" s="19"/>
       <c r="AY38" s="8"/>
+      <c r="BA38" s="40" t="s">
+        <v>633</v>
+      </c>
+      <c r="BB38" s="41"/>
+      <c r="BC38" s="40" t="s">
+        <v>634</v>
+      </c>
+      <c r="BD38" s="41"/>
+      <c r="BE38" s="40" t="s">
+        <v>427</v>
+      </c>
+      <c r="BG38" s="40" t="s">
+        <v>569</v>
+      </c>
+      <c r="BH38" s="41"/>
+      <c r="BI38" s="41"/>
       <c r="BK38" s="2" t="s">
         <v>464</v>
       </c>

</xml_diff>

<commit_message>
Asset list and level update
</commit_message>
<xml_diff>
--- a/Planning/Assetlist.xlsx
+++ b/Planning/Assetlist.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carloakuma\Desktop\Gamelab1\Planning\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="4368"/>
   </bookViews>
@@ -29,7 +24,7 @@
     <author>CarloAkuma</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="676">
   <si>
     <t>2D</t>
   </si>
@@ -2056,12 +2051,42 @@
   </si>
   <si>
     <t>knoop</t>
+  </si>
+  <si>
+    <t>2D_ENVBRO_001</t>
+  </si>
+  <si>
+    <t>20 minuten</t>
+  </si>
+  <si>
+    <t>2D_ENVKRANT_001</t>
+  </si>
+  <si>
+    <t>1 uur</t>
+  </si>
+  <si>
+    <t>3D_ENVBRO</t>
+  </si>
+  <si>
+    <t>Broom</t>
+  </si>
+  <si>
+    <t>Krant</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <t>3D_ENVKRANT_001</t>
+  </si>
+  <si>
+    <t>_001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2266,7 +2291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2310,9 +2335,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2582,7 +2609,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2592,8 +2619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:CD110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E101" sqref="E101"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P78" sqref="P78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9232,7 +9259,22 @@
       </c>
       <c r="I76" s="21"/>
       <c r="J76" s="21"/>
+      <c r="L76" s="44" t="s">
+        <v>670</v>
+      </c>
+      <c r="M76" t="s">
+        <v>675</v>
+      </c>
+      <c r="N76" s="44" t="s">
+        <v>671</v>
+      </c>
+      <c r="P76" t="s">
+        <v>170</v>
+      </c>
       <c r="Q76" s="36"/>
+      <c r="R76" s="44" t="s">
+        <v>673</v>
+      </c>
       <c r="T76" s="21"/>
       <c r="AD76" s="21"/>
     </row>
@@ -9254,6 +9296,18 @@
       </c>
       <c r="I77" s="21"/>
       <c r="J77" s="21"/>
+      <c r="L77" s="37" t="s">
+        <v>674</v>
+      </c>
+      <c r="N77" s="37" t="s">
+        <v>672</v>
+      </c>
+      <c r="P77" t="s">
+        <v>170</v>
+      </c>
+      <c r="R77" s="37" t="s">
+        <v>581</v>
+      </c>
       <c r="T77" s="21"/>
       <c r="AD77" s="21"/>
     </row>
@@ -9587,6 +9641,34 @@
       <c r="G93" s="12"/>
       <c r="H93" s="20" t="s">
         <v>576</v>
+      </c>
+    </row>
+    <row r="94" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B94" s="43" t="s">
+        <v>666</v>
+      </c>
+      <c r="D94" s="43" t="s">
+        <v>671</v>
+      </c>
+      <c r="F94" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="H94" s="20" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="95" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>668</v>
+      </c>
+      <c r="D95" s="43" t="s">
+        <v>672</v>
+      </c>
+      <c r="F95" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="H95" s="20" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>